<commit_message>
first run for Kenya - dr and dridv missing
</commit_message>
<xml_diff>
--- a/workflow/1_Experiment/0_From_Confection/B1_Model_Structure.xlsx
+++ b/workflow/1_Experiment/0_From_Confection/B1_Model_Structure.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="314">
   <si>
     <t>set</t>
   </si>
@@ -111,79 +111,373 @@
     <t>u</t>
   </si>
   <si>
-    <t>RSA_POW_TD</t>
-  </si>
-  <si>
-    <t>RSA_FUEL_PRO_COAL</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_COAL</t>
-  </si>
-  <si>
-    <t>RSA_POW_INT</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_NU_OLD</t>
-  </si>
-  <si>
-    <t>RSA_FUEL_PRO_URNM</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_MMG</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_PEAK</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_BIOM</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_HYDR</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_CSP</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_PV_UT</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_PV_DIST</t>
-  </si>
-  <si>
-    <t>RSA_FUEL_PRO_NG</t>
-  </si>
-  <si>
-    <t>RSA_FUEL_PRO_BIOM</t>
-  </si>
-  <si>
-    <t>RSA_POW_ELEC</t>
-  </si>
-  <si>
-    <t>RSA_FUEL_PRO_DSL</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_BST</t>
-  </si>
-  <si>
-    <t>RSA_POW_STO_BAT_IN</t>
-  </si>
-  <si>
-    <t>RSA_POW_STO_BAT_OUT</t>
-  </si>
-  <si>
-    <t>RSA_POW_STO_PHY_IN</t>
-  </si>
-  <si>
-    <t>RSA_POW_STO_PHY_OUT</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_NU</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_NU_SMR</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_WIND</t>
+    <t>BACKSTOP</t>
+  </si>
+  <si>
+    <t>BESS_TECH</t>
+  </si>
+  <si>
+    <t>DEMCOMELC</t>
+  </si>
+  <si>
+    <t>DEMINDELC</t>
+  </si>
+  <si>
+    <t>DEMRESELC</t>
+  </si>
+  <si>
+    <t>EXPELC</t>
+  </si>
+  <si>
+    <t>IMPBIO</t>
+  </si>
+  <si>
+    <t>IMPCOA</t>
+  </si>
+  <si>
+    <t>IMPELC001</t>
+  </si>
+  <si>
+    <t>IMPELC002</t>
+  </si>
+  <si>
+    <t>IMPHFOMOM</t>
+  </si>
+  <si>
+    <t>IMPHFONAI</t>
+  </si>
+  <si>
+    <t>IMPLFOELD</t>
+  </si>
+  <si>
+    <t>IMPNGS</t>
+  </si>
+  <si>
+    <t>IMPURN</t>
+  </si>
+  <si>
+    <t>MINBIO</t>
+  </si>
+  <si>
+    <t>MINCOA</t>
+  </si>
+  <si>
+    <t>MINGEO</t>
+  </si>
+  <si>
+    <t>MINHYD</t>
+  </si>
+  <si>
+    <t>MINSOL</t>
+  </si>
+  <si>
+    <t>MINWND</t>
+  </si>
+  <si>
+    <t>PWRBIO001</t>
+  </si>
+  <si>
+    <t>PWRCOA001</t>
+  </si>
+  <si>
+    <t>PWRDIST</t>
+  </si>
+  <si>
+    <t>PWRGEO001</t>
+  </si>
+  <si>
+    <t>PWRGEO002</t>
+  </si>
+  <si>
+    <t>PWRGEO003</t>
+  </si>
+  <si>
+    <t>PWRGEO004</t>
+  </si>
+  <si>
+    <t>PWRGEO005</t>
+  </si>
+  <si>
+    <t>PWRGEO006</t>
+  </si>
+  <si>
+    <t>PWRGEO007</t>
+  </si>
+  <si>
+    <t>PWRHFO001</t>
+  </si>
+  <si>
+    <t>PWRHYD001</t>
+  </si>
+  <si>
+    <t>PWRHYD002</t>
+  </si>
+  <si>
+    <t>PWRHYD003</t>
+  </si>
+  <si>
+    <t>PWRHYD004</t>
+  </si>
+  <si>
+    <t>PWRHYD005</t>
+  </si>
+  <si>
+    <t>PWRLFO001</t>
+  </si>
+  <si>
+    <t>PWRNGS001</t>
+  </si>
+  <si>
+    <t>PWRPHS001</t>
+  </si>
+  <si>
+    <t>PWRPHS002</t>
+  </si>
+  <si>
+    <t>PWRSOL001</t>
+  </si>
+  <si>
+    <t>PWRSOL002</t>
+  </si>
+  <si>
+    <t>PWRTRN</t>
+  </si>
+  <si>
+    <t>PWRURN001</t>
+  </si>
+  <si>
+    <t>PWRWND001</t>
+  </si>
+  <si>
+    <t>PWRWND002</t>
+  </si>
+  <si>
+    <t>PWRWND003</t>
+  </si>
+  <si>
+    <t>PWRWND004</t>
+  </si>
+  <si>
+    <t>PWRWND005</t>
+  </si>
+  <si>
+    <t>PWRWND006</t>
+  </si>
+  <si>
+    <t>PWRWND007</t>
+  </si>
+  <si>
+    <t>PWRWND008</t>
+  </si>
+  <si>
+    <t>PWRWND009</t>
+  </si>
+  <si>
+    <t>PWRWND010</t>
+  </si>
+  <si>
+    <t>PWRWND011</t>
+  </si>
+  <si>
+    <t>TS01</t>
+  </si>
+  <si>
+    <t>TS02</t>
+  </si>
+  <si>
+    <t>TS03</t>
+  </si>
+  <si>
+    <t>TS04</t>
+  </si>
+  <si>
+    <t>TS05</t>
+  </si>
+  <si>
+    <t>TS06</t>
+  </si>
+  <si>
+    <t>TS07</t>
+  </si>
+  <si>
+    <t>TS08</t>
+  </si>
+  <si>
+    <t>TS09</t>
+  </si>
+  <si>
+    <t>TS10</t>
+  </si>
+  <si>
+    <t>TS11</t>
+  </si>
+  <si>
+    <t>TS12</t>
+  </si>
+  <si>
+    <t>TS13</t>
+  </si>
+  <si>
+    <t>TS14</t>
+  </si>
+  <si>
+    <t>TS15</t>
+  </si>
+  <si>
+    <t>TS16</t>
+  </si>
+  <si>
+    <t>TS17</t>
+  </si>
+  <si>
+    <t>TS18</t>
+  </si>
+  <si>
+    <t>TS19</t>
+  </si>
+  <si>
+    <t>TS20</t>
+  </si>
+  <si>
+    <t>TS21</t>
+  </si>
+  <si>
+    <t>TS22</t>
+  </si>
+  <si>
+    <t>TS23</t>
+  </si>
+  <si>
+    <t>TS24</t>
+  </si>
+  <si>
+    <t>TS25</t>
+  </si>
+  <si>
+    <t>TS26</t>
+  </si>
+  <si>
+    <t>TS27</t>
+  </si>
+  <si>
+    <t>TS28</t>
+  </si>
+  <si>
+    <t>TS29</t>
+  </si>
+  <si>
+    <t>TS30</t>
+  </si>
+  <si>
+    <t>TS31</t>
+  </si>
+  <si>
+    <t>TS32</t>
+  </si>
+  <si>
+    <t>TS33</t>
+  </si>
+  <si>
+    <t>TS34</t>
+  </si>
+  <si>
+    <t>TS35</t>
+  </si>
+  <si>
+    <t>TS36</t>
+  </si>
+  <si>
+    <t>TS37</t>
+  </si>
+  <si>
+    <t>TS38</t>
+  </si>
+  <si>
+    <t>TS39</t>
+  </si>
+  <si>
+    <t>TS40</t>
+  </si>
+  <si>
+    <t>TS41</t>
+  </si>
+  <si>
+    <t>TS42</t>
+  </si>
+  <si>
+    <t>TS43</t>
+  </si>
+  <si>
+    <t>TS44</t>
+  </si>
+  <si>
+    <t>TS45</t>
+  </si>
+  <si>
+    <t>TS46</t>
+  </si>
+  <si>
+    <t>TS47</t>
+  </si>
+  <si>
+    <t>TS48</t>
+  </si>
+  <si>
+    <t>BIO</t>
+  </si>
+  <si>
+    <t>COA</t>
+  </si>
+  <si>
+    <t>COADOM</t>
+  </si>
+  <si>
+    <t>COMELC</t>
+  </si>
+  <si>
+    <t>ELC001</t>
+  </si>
+  <si>
+    <t>ELC002</t>
+  </si>
+  <si>
+    <t>ELC003</t>
+  </si>
+  <si>
+    <t>GEO</t>
+  </si>
+  <si>
+    <t>HFOMOM</t>
+  </si>
+  <si>
+    <t>HFONAI</t>
+  </si>
+  <si>
+    <t>HYD</t>
+  </si>
+  <si>
+    <t>INDELC</t>
+  </si>
+  <si>
+    <t>LFOELD</t>
+  </si>
+  <si>
+    <t>NGS</t>
+  </si>
+  <si>
+    <t>RESELC</t>
+  </si>
+  <si>
+    <t>SOL</t>
+  </si>
+  <si>
+    <t>URN</t>
+  </si>
+  <si>
+    <t>WND</t>
+  </si>
+  <si>
+    <t>CO2</t>
   </si>
   <si>
     <t>1</t>
@@ -192,6 +486,9 @@
     <t>2</t>
   </si>
   <si>
+    <t>RE1</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
@@ -204,208 +501,13 @@
     <t>6</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>RSA_POW_ELE</t>
-  </si>
-  <si>
-    <t>RSA_POW_ELEF</t>
-  </si>
-  <si>
-    <t>RSA_POW_ELEX</t>
-  </si>
-  <si>
-    <t>RSA_POW_H2</t>
-  </si>
-  <si>
-    <t>RSA_FUEL_URNM</t>
-  </si>
-  <si>
-    <t>RSA_FUEL_COAL</t>
-  </si>
-  <si>
-    <t>RSA_FUEL_NG</t>
-  </si>
-  <si>
-    <t>RSA_FUEL_DSL</t>
-  </si>
-  <si>
-    <t>RSA_FUEL_BIOM</t>
-  </si>
-  <si>
-    <t>RSA_POW_NUEL</t>
-  </si>
-  <si>
-    <t>RSA_CO2</t>
-  </si>
-  <si>
-    <t>RE1</t>
-  </si>
-  <si>
-    <t>RSA_POW_STO_BAT</t>
-  </si>
-  <si>
-    <t>RSA_POW_STO_PHY</t>
-  </si>
-  <si>
-    <t>RSA_POW_STO_H2</t>
-  </si>
-  <si>
-    <t>RESMAR</t>
-  </si>
-  <si>
-    <t>MINLFSMR</t>
-  </si>
-  <si>
-    <t>MINLFPEAK</t>
-  </si>
-  <si>
-    <t>MINLFMMG</t>
-  </si>
-  <si>
-    <t>MINLFCOAL</t>
+    <t>BESS001</t>
+  </si>
+  <si>
+    <t>PHS001</t>
+  </si>
+  <si>
+    <t>PHS002</t>
   </si>
   <si>
     <t>category</t>
@@ -1187,7 +1289,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1292,16 +1394,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="D3">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1313,7 +1415,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1331,589 +1433,647 @@
         <v>2</v>
       </c>
       <c r="O3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="B4">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="F4" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>154</v>
       </c>
       <c r="H4" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>154</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>154</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
+        <v>154</v>
       </c>
       <c r="L4" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="M4" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="N4" t="s">
-        <v>123</v>
-      </c>
-      <c r="O4" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="B5">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="K5" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="L5" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="N5" t="s">
-        <v>124</v>
-      </c>
-      <c r="O5" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="B6">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>157</v>
       </c>
       <c r="K6" t="s">
-        <v>58</v>
+        <v>157</v>
       </c>
       <c r="L6" t="s">
-        <v>124</v>
-      </c>
-      <c r="O6" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="B7">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>158</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
-      </c>
-      <c r="O7" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="B8">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C8" t="s">
         <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
-      </c>
-      <c r="I8" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="K8" t="s">
-        <v>60</v>
-      </c>
-      <c r="O8" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="B9">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C9" t="s">
         <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="K9" t="s">
-        <v>61</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="B10">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="B11">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="B12">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="E12" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="B13">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="E13" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="B14">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="B15">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="C15" t="s">
         <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="B16">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="C16" t="s">
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
       <c r="B17">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
+        <v>100</v>
+      </c>
+      <c r="E17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
       <c r="B18">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="C18" t="s">
         <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
+        <v>101</v>
+      </c>
+      <c r="E18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
       <c r="B19">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="C19" t="s">
         <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
+        <v>102</v>
+      </c>
+      <c r="E19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
+        <v>103</v>
+      </c>
+      <c r="E20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
       <c r="B21">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
       <c r="B22">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="C22" t="s">
         <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
       <c r="B23">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="C23" t="s">
         <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
       <c r="B24">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="C24" t="s">
         <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="C26" t="s">
         <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
       <c r="B27">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C27" t="s">
         <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
       <c r="B28">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="C28" t="s">
         <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
       <c r="B29">
+        <v>2044</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30">
         <v>2045</v>
       </c>
-      <c r="D29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30">
+      <c r="C30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31">
         <v>2046</v>
       </c>
-      <c r="D30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31">
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32">
         <v>2047</v>
       </c>
-      <c r="D31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32">
-        <v>2048</v>
+      <c r="C32" t="s">
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33">
-        <v>2049</v>
+        <v>2048</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34">
-        <v>2050</v>
+        <v>2049</v>
+      </c>
+      <c r="C34" t="s">
+        <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35">
-        <v>2051</v>
+        <v>2050</v>
+      </c>
+      <c r="C35" t="s">
+        <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36">
-        <v>2052</v>
+      <c r="C36" t="s">
+        <v>63</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37">
-        <v>2053</v>
+      <c r="C37" t="s">
+        <v>64</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="2:4">
-      <c r="B38">
-        <v>2054</v>
+      <c r="C38" t="s">
+        <v>65</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="2:4">
-      <c r="B39">
-        <v>2055</v>
+      <c r="C39" t="s">
+        <v>66</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40">
-        <v>2056</v>
+      <c r="C40" t="s">
+        <v>67</v>
       </c>
       <c r="D40" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="2:4">
-      <c r="B41">
-        <v>2057</v>
+      <c r="C41" t="s">
+        <v>68</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="2:4">
-      <c r="B42">
-        <v>2058</v>
+      <c r="C42" t="s">
+        <v>69</v>
       </c>
       <c r="D42" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="2:4">
-      <c r="B43">
-        <v>2059</v>
+      <c r="C43" t="s">
+        <v>70</v>
       </c>
       <c r="D43" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="2:4">
-      <c r="B44">
-        <v>2060</v>
+      <c r="C44" t="s">
+        <v>71</v>
       </c>
       <c r="D44" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="2:4">
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
       <c r="D45" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="2:4">
+      <c r="C46" t="s">
+        <v>73</v>
+      </c>
       <c r="D46" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="2:4">
+      <c r="C47" t="s">
+        <v>74</v>
+      </c>
       <c r="D47" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="2:4">
+      <c r="C48" t="s">
+        <v>75</v>
+      </c>
       <c r="D48" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4">
+      <c r="C49" t="s">
+        <v>76</v>
+      </c>
       <c r="D49" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4">
+      <c r="C50" t="s">
+        <v>77</v>
+      </c>
       <c r="D50" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4">
+      <c r="C51" t="s">
+        <v>78</v>
+      </c>
       <c r="D51" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4">
-      <c r="D52" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4">
-      <c r="D53" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4">
-      <c r="D54" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4">
-      <c r="D55" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4">
-      <c r="D56" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4">
-      <c r="D57" t="s">
-        <v>109</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4">
+      <c r="C52" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4">
+      <c r="C53" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4">
+      <c r="C54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4">
+      <c r="C55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4">
+      <c r="C56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4">
+      <c r="C57" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4">
+      <c r="C58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4">
+      <c r="C59" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1931,37 +2091,37 @@
   <sheetData>
     <row r="1" spans="1:69">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="L1" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="O1" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="AA1" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="AE1" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="AI1" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="AM1" t="s">
-        <v>176</v>
+        <v>210</v>
       </c>
       <c r="AP1" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="AS1" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
       <c r="AZ1" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
       <c r="BM1" t="s">
         <v>16</v>
@@ -1969,211 +2129,211 @@
     </row>
     <row r="2" spans="1:69">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="G2" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="H2" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="I2" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="J2" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="K2" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="L2" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="M2" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="N2" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="O2" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="P2" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="Q2" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="R2" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="S2" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
       <c r="T2" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
       <c r="U2" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="V2" t="s">
-        <v>156</v>
+        <v>190</v>
       </c>
       <c r="W2" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="X2" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="Y2" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="Z2" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
       <c r="AA2" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
       <c r="AB2" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="AC2" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="AD2" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="AE2" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="AF2" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="AG2" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="AH2" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="AI2" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="AJ2" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="AK2" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="AL2" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="AM2" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="AN2" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="AO2" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="AP2" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="AQ2" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
       <c r="AR2" t="s">
-        <v>183</v>
+        <v>217</v>
       </c>
       <c r="AS2" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="AT2" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="AU2" t="s">
-        <v>187</v>
+        <v>221</v>
       </c>
       <c r="AV2" t="s">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="AW2" t="s">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="AX2" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
       <c r="AY2" t="s">
-        <v>191</v>
+        <v>225</v>
       </c>
       <c r="AZ2" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="BA2" t="s">
-        <v>194</v>
+        <v>228</v>
       </c>
       <c r="BB2" t="s">
-        <v>195</v>
+        <v>229</v>
       </c>
       <c r="BC2" t="s">
-        <v>196</v>
+        <v>230</v>
       </c>
       <c r="BD2" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="BE2" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="BF2" t="s">
+        <v>233</v>
+      </c>
+      <c r="BG2" t="s">
         <v>199</v>
       </c>
-      <c r="BG2" t="s">
-        <v>165</v>
-      </c>
       <c r="BH2" t="s">
-        <v>200</v>
+        <v>234</v>
       </c>
       <c r="BI2" t="s">
-        <v>201</v>
+        <v>235</v>
       </c>
       <c r="BJ2" t="s">
-        <v>202</v>
+        <v>236</v>
       </c>
       <c r="BK2" t="s">
-        <v>203</v>
+        <v>237</v>
       </c>
       <c r="BL2" t="s">
-        <v>204</v>
+        <v>238</v>
       </c>
       <c r="BM2" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
       <c r="BN2" t="s">
-        <v>206</v>
+        <v>240</v>
       </c>
       <c r="BO2" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="BP2" t="s">
-        <v>208</v>
+        <v>242</v>
       </c>
       <c r="BQ2" t="s">
-        <v>209</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:69">
@@ -2599,7 +2759,7 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
@@ -3016,228 +3176,228 @@
   <sheetData>
     <row r="1" spans="1:66">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="D1" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="J1" t="s">
-        <v>220</v>
+        <v>254</v>
       </c>
       <c r="AA1" t="s">
-        <v>238</v>
+        <v>272</v>
       </c>
       <c r="AK1" t="s">
-        <v>176</v>
+        <v>210</v>
       </c>
       <c r="AV1" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
       <c r="BM1" t="s">
-        <v>277</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:66">
       <c r="A2" t="s">
-        <v>210</v>
+        <v>244</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>245</v>
       </c>
       <c r="C2" t="s">
-        <v>212</v>
+        <v>246</v>
       </c>
       <c r="D2" t="s">
-        <v>214</v>
+        <v>248</v>
       </c>
       <c r="E2" t="s">
-        <v>215</v>
+        <v>249</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
+        <v>250</v>
       </c>
       <c r="G2" t="s">
-        <v>217</v>
+        <v>251</v>
       </c>
       <c r="H2" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="I2" t="s">
-        <v>219</v>
+        <v>253</v>
       </c>
       <c r="J2" t="s">
-        <v>221</v>
+        <v>255</v>
       </c>
       <c r="K2" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
       <c r="L2" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="M2" t="s">
-        <v>224</v>
+        <v>258</v>
       </c>
       <c r="N2" t="s">
-        <v>225</v>
+        <v>259</v>
       </c>
       <c r="O2" t="s">
-        <v>226</v>
+        <v>260</v>
       </c>
       <c r="P2" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="Q2" t="s">
-        <v>228</v>
+        <v>262</v>
       </c>
       <c r="R2" t="s">
-        <v>229</v>
+        <v>263</v>
       </c>
       <c r="S2" t="s">
-        <v>230</v>
+        <v>264</v>
       </c>
       <c r="T2" t="s">
-        <v>231</v>
+        <v>265</v>
       </c>
       <c r="U2" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="V2" t="s">
-        <v>233</v>
+        <v>267</v>
       </c>
       <c r="W2" t="s">
-        <v>234</v>
+        <v>268</v>
       </c>
       <c r="X2" t="s">
-        <v>235</v>
+        <v>269</v>
       </c>
       <c r="Y2" t="s">
-        <v>236</v>
+        <v>270</v>
       </c>
       <c r="Z2" t="s">
-        <v>237</v>
+        <v>271</v>
       </c>
       <c r="AA2" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="AB2" t="s">
-        <v>240</v>
+        <v>274</v>
       </c>
       <c r="AC2" t="s">
-        <v>241</v>
+        <v>275</v>
       </c>
       <c r="AD2" t="s">
-        <v>242</v>
+        <v>276</v>
       </c>
       <c r="AE2" t="s">
-        <v>243</v>
+        <v>277</v>
       </c>
       <c r="AF2" t="s">
-        <v>244</v>
+        <v>278</v>
       </c>
       <c r="AG2" t="s">
-        <v>245</v>
+        <v>279</v>
       </c>
       <c r="AH2" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
       <c r="AI2" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
       <c r="AJ2" t="s">
-        <v>248</v>
+        <v>282</v>
       </c>
       <c r="AK2" t="s">
-        <v>249</v>
+        <v>283</v>
       </c>
       <c r="AL2" t="s">
-        <v>250</v>
+        <v>284</v>
       </c>
       <c r="AM2" t="s">
-        <v>251</v>
+        <v>285</v>
       </c>
       <c r="AN2" t="s">
-        <v>252</v>
+        <v>286</v>
       </c>
       <c r="AO2" t="s">
-        <v>253</v>
+        <v>287</v>
       </c>
       <c r="AP2" t="s">
-        <v>254</v>
+        <v>288</v>
       </c>
       <c r="AQ2" t="s">
-        <v>255</v>
+        <v>289</v>
       </c>
       <c r="AR2" t="s">
-        <v>256</v>
+        <v>290</v>
       </c>
       <c r="AS2" t="s">
-        <v>257</v>
+        <v>291</v>
       </c>
       <c r="AT2" t="s">
-        <v>258</v>
+        <v>292</v>
       </c>
       <c r="AU2" t="s">
-        <v>259</v>
+        <v>293</v>
       </c>
       <c r="AV2" t="s">
-        <v>260</v>
+        <v>294</v>
       </c>
       <c r="AW2" t="s">
-        <v>261</v>
+        <v>295</v>
       </c>
       <c r="AX2" t="s">
-        <v>262</v>
+        <v>296</v>
       </c>
       <c r="AY2" t="s">
-        <v>263</v>
+        <v>297</v>
       </c>
       <c r="AZ2" t="s">
-        <v>264</v>
+        <v>298</v>
       </c>
       <c r="BA2" t="s">
-        <v>265</v>
+        <v>299</v>
       </c>
       <c r="BB2" t="s">
-        <v>266</v>
+        <v>300</v>
       </c>
       <c r="BC2" t="s">
-        <v>267</v>
+        <v>301</v>
       </c>
       <c r="BD2" t="s">
-        <v>268</v>
+        <v>302</v>
       </c>
       <c r="BE2" t="s">
-        <v>269</v>
+        <v>303</v>
       </c>
       <c r="BF2" t="s">
-        <v>270</v>
+        <v>304</v>
       </c>
       <c r="BG2" t="s">
-        <v>271</v>
+        <v>305</v>
       </c>
       <c r="BH2" t="s">
-        <v>272</v>
+        <v>306</v>
       </c>
       <c r="BI2" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="BJ2" t="s">
-        <v>274</v>
+        <v>308</v>
       </c>
       <c r="BK2" t="s">
-        <v>275</v>
+        <v>309</v>
       </c>
       <c r="BL2" t="s">
-        <v>276</v>
+        <v>310</v>
       </c>
       <c r="BM2" t="s">
-        <v>278</v>
+        <v>312</v>
       </c>
       <c r="BN2" t="s">
-        <v>279</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:66">
@@ -3711,7 +3871,7 @@
         <v>20</v>
       </c>
       <c r="Z5" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="AA5" t="s">
         <v>18</v>

</xml_diff>